<commit_message>
Added CFG tests in JUnit 5
</commit_message>
<xml_diff>
--- a/docs/lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/docs/lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF45495-1424-49E3-B431-4DCD0C3AADE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D319871F-FFB5-4CF3-87C4-1CE0EB529451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -575,12 +575,36 @@
   <si>
     <t>F02. Afisarea task-urilor planificate intr-o anumita perioada de timp, precizata ca data si ora de inceput si data si ora de sfarsit.</t>
   </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>[[task activ, nerepetitiv cu start=03/04/2022 12:00]]</t>
+  </si>
+  <si>
+    <t>[task activ, nerepetitiv cu start=03/04/2022 12:00]</t>
+  </si>
+  <si>
+    <t>[task activ, repetitiv cu start=04/04/2022 12:00]</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, repetitiv cu start=03/04/2022 12:00]</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,6 +745,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -791,12 +821,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor rgb="FF8DB3E2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -877,19 +907,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1147,19 +1164,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -1216,17 +1220,6 @@
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1285,11 +1278,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="double">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="double">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1298,76 +1416,60 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1376,32 +1478,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="7" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="7" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="7" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1412,182 +1545,173 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2002,16 +2126,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="12"/>
-      <c r="D1" s="40" t="s">
+      <c r="B1" s="9"/>
+      <c r="D1" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="33" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2019,31 +2143,31 @@
       <c r="B4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27" t="s">
+      <c r="N6" s="21"/>
+      <c r="O6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="21" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2052,13 +2176,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="27" t="s">
+      <c r="N7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="27" t="s">
+      <c r="O7" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="P7" s="27">
+      <c r="P7" s="21">
         <v>235</v>
       </c>
     </row>
@@ -2067,13 +2191,13 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="27" t="s">
+      <c r="N8" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="O8" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="27">
+      <c r="P8" s="21">
         <v>235</v>
       </c>
     </row>
@@ -2084,13 +2208,13 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="27" t="s">
+      <c r="N9" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="O9" s="27" t="s">
+      <c r="O9" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="27">
+      <c r="P9" s="21">
         <v>235</v>
       </c>
     </row>
@@ -2103,7 +2227,7 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="31" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="1"/>
@@ -2149,353 +2273,353 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B1" s="12"/>
-      <c r="D1" s="40" t="s">
+      <c r="B1" s="9"/>
+      <c r="D1" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="I6" s="40" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="I6" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="Q6" s="40" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="Q6" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="I8" s="12" t="s">
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="I8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="45" t="s">
+      <c r="Q8" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="34">
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="28">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="I9" s="38"/>
-      <c r="Q9" s="45" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="I9" s="32"/>
+      <c r="Q9" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="34" t="s">
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="28" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="I10" s="49" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="I10" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
-      <c r="Q10" s="45" t="s">
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="55"/>
+      <c r="Q10" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="R10" s="45" t="s">
+      <c r="R10" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="45"/>
-      <c r="T10" s="34" t="s">
+      <c r="S10" s="49"/>
+      <c r="T10" s="28" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="54"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="58"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="58"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="54"/>
-      <c r="Q13" s="40" t="s">
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="58"/>
+      <c r="Q13" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="54"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="58"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I15" s="52"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="54"/>
-      <c r="Q15" s="32" t="s">
+      <c r="I15" s="56"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="58"/>
+      <c r="Q15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="58" t="s">
+      <c r="R15" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="54"/>
-      <c r="Q16" s="35" t="s">
+      <c r="I16" s="56"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="58"/>
+      <c r="Q16" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="R16" s="43" t="s">
+      <c r="R16" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I17" s="52"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="54"/>
-      <c r="Q17" s="35" t="s">
+      <c r="I17" s="56"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="58"/>
+      <c r="Q17" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="R17" s="43" t="s">
+      <c r="R17" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="54"/>
-      <c r="Q18" s="35" t="s">
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="58"/>
+      <c r="Q18" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="R18" s="43" t="s">
+      <c r="R18" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="47"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="e">
         <f>- R19</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="54"/>
-      <c r="Q19" s="35" t="s">
+      <c r="I19" s="56"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="58"/>
+      <c r="Q19" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="R19" s="43" t="s">
+      <c r="R19" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="S19" s="43"/>
-      <c r="T19" s="43"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I20" s="52"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="54"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="58"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="52"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="54"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="58"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="52"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="54"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="58"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I23" s="52"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="54"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="58"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I24" s="55"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="57"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -2515,6 +2639,7 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R18:T18"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="R16:T16"/>
@@ -2522,7 +2647,6 @@
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="Q13:T13"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="R18:T18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2537,7 +2661,7 @@
   </sheetPr>
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -2562,518 +2686,518 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B1" s="12"/>
-      <c r="D1" s="40" t="s">
+      <c r="B1" s="9"/>
+      <c r="D1" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="6" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="D6" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="65"/>
-      <c r="AA6" s="65"/>
-      <c r="AB6" s="65"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="70"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="70"/>
+      <c r="W6" s="70"/>
+      <c r="X6" s="70"/>
+      <c r="Y6" s="70"/>
+      <c r="Z6" s="70"/>
+      <c r="AA6" s="70"/>
+      <c r="AB6" s="70"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="62" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="F7" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
-      <c r="O7" s="61"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="63" t="s">
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="S7" s="63"/>
-      <c r="T7" s="63"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="64" t="s">
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="68"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
     </row>
     <row r="8" spans="2:28" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="65"/>
-      <c r="C8" s="59" t="s">
+      <c r="B8" s="70"/>
+      <c r="C8" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="61" t="s">
+      <c r="E8" s="66"/>
+      <c r="F8" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61" t="s">
+      <c r="G8" s="65"/>
+      <c r="H8" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61" t="s">
+      <c r="I8" s="65"/>
+      <c r="J8" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61" t="s">
+      <c r="K8" s="65"/>
+      <c r="L8" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61" t="s">
+      <c r="M8" s="65"/>
+      <c r="N8" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="O8" s="61"/>
-      <c r="P8" s="61" t="s">
+      <c r="O8" s="65"/>
+      <c r="P8" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="Q8" s="61"/>
-      <c r="R8" s="63" t="s">
+      <c r="Q8" s="65"/>
+      <c r="R8" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="S8" s="63" t="s">
+      <c r="S8" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="63" t="s">
+      <c r="T8" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="U8" s="63" t="s">
+      <c r="U8" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="V8" s="64">
+      <c r="V8" s="68">
         <v>0</v>
       </c>
-      <c r="W8" s="64">
+      <c r="W8" s="68">
         <v>1</v>
       </c>
-      <c r="X8" s="64">
+      <c r="X8" s="68">
         <v>2</v>
       </c>
-      <c r="Y8" s="64" t="s">
+      <c r="Y8" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="Z8" s="64" t="s">
+      <c r="Z8" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="AA8" s="64" t="s">
+      <c r="AA8" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="AB8" s="64" t="s">
+      <c r="AB8" s="68" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="65"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="13" t="s">
+      <c r="B9" s="70"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="O9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="P9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" s="13" t="s">
+      <c r="Q9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="63"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="64"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="67"/>
+      <c r="U9" s="67"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="68"/>
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="68"/>
     </row>
     <row r="10" spans="2:28" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="107" t="s">
+      <c r="C10" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="18" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="19" t="s">
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="16"/>
     </row>
     <row r="11" spans="2:28" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18" t="s">
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="19" t="s">
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="19"/>
-      <c r="AB11" s="19"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
     </row>
     <row r="12" spans="2:28" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="109" t="s">
+      <c r="D12" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17" t="s">
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18" t="s">
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19" t="s">
+      <c r="U12" s="15"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="AA12" s="19"/>
-      <c r="AB12" s="19"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="16"/>
     </row>
     <row r="13" spans="2:28" ht="111" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="108" t="s">
+      <c r="C13" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17" t="s">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17" t="s">
+      <c r="I13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17" t="s">
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17" t="s">
+      <c r="N13" s="14"/>
+      <c r="O13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17" t="s">
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18" t="s">
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="U13" s="18"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19" t="s">
+      <c r="U13" s="15"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="16"/>
     </row>
     <row r="14" spans="2:28" ht="111" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17" t="s">
+      <c r="I14" s="14"/>
+      <c r="J14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17" t="s">
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17" t="s">
+      <c r="O14" s="14"/>
+      <c r="P14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18" t="s">
+      <c r="Q14" s="14"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19" t="s">
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="19"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
     </row>
     <row r="15" spans="2:28" ht="111" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17" t="s">
+      <c r="I15" s="14"/>
+      <c r="J15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17" t="s">
+      <c r="K15" s="14"/>
+      <c r="L15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17" t="s">
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P15" s="17" t="s">
+      <c r="P15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18" t="s">
+      <c r="Q15" s="14"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19" t="s">
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
     </row>
     <row r="16" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
+      <c r="B16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -3093,9 +3217,6 @@
     <mergeCell ref="V7:AB7"/>
     <mergeCell ref="AB8:AB9"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
     <mergeCell ref="V8:V9"/>
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="S8:S9"/>
@@ -3106,6 +3227,9 @@
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:Q7"/>
     <mergeCell ref="R7:U7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3117,10 +3241,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,416 +3253,367 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="12"/>
-      <c r="D1" s="40" t="s">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B1" s="9"/>
+      <c r="D1" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="93" t="s">
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="94" t="s">
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="87" t="s">
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="88"/>
-    </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="95"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="101"/>
+      <c r="I4" s="102"/>
+    </row>
+    <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="100"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="106"/>
       <c r="E5" s="2" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="90"/>
-      <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21">
+    <row r="6" spans="2:24" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="107">
         <v>9</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="38">
+        <v>44653.5</v>
+      </c>
+      <c r="G6" s="38">
+        <v>44652.5</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="18"/>
+    </row>
+    <row r="7" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="108">
+        <v>10</v>
+      </c>
+      <c r="C7" s="111"/>
+      <c r="D7" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="40">
+        <v>44653.5</v>
+      </c>
+      <c r="G7" s="40">
+        <v>44654.5</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="L7" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="76"/>
+      <c r="R7" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="92"/>
+      <c r="W7" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="X7" s="97"/>
+    </row>
+    <row r="8" spans="2:24" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="108">
+        <v>11</v>
+      </c>
+      <c r="C8" s="111"/>
+      <c r="D8" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="40">
+        <v>44653.5</v>
+      </c>
+      <c r="G8" s="40">
+        <v>44654.5</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="L8" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="89" t="s">
+        <v>70</v>
+      </c>
+      <c r="P8" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q8" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="R8" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="S8" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="T8" s="82" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="W8" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="X8" s="78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="108">
+        <v>12</v>
+      </c>
+      <c r="C9" s="111"/>
+      <c r="D9" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="40">
+        <v>44653.5</v>
+      </c>
+      <c r="G9" s="40">
+        <v>44654.5</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="L9" s="87"/>
+      <c r="M9" s="88"/>
+      <c r="N9" s="88"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="91"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="83"/>
+      <c r="T9" s="83"/>
+      <c r="U9" s="85"/>
+      <c r="V9" s="94"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="79"/>
+    </row>
+    <row r="10" spans="2:24" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="108">
+        <v>13</v>
+      </c>
+      <c r="C10" s="111"/>
+      <c r="D10" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="40">
+        <v>44653.5</v>
+      </c>
+      <c r="G10" s="40">
+        <v>44655.5</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="L10" s="21">
+        <f>SUM(M10:N10)</f>
         <v>6</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="85" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="86"/>
-      <c r="K6" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="21">
-        <v>10</v>
-      </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="21">
-        <v>5</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="M10" s="19">
         <v>6</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="N10" s="19">
+        <v>0</v>
+      </c>
+      <c r="O10" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="P10" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" s="21">
+        <f>SUM(T10:U10)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="19">
+        <v>0</v>
+      </c>
+      <c r="U10" s="22">
+        <v>0</v>
+      </c>
+      <c r="V10" s="23"/>
+      <c r="W10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="X10" s="24">
+        <f>M10</f>
         <v>6</v>
       </c>
-      <c r="H7" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="88"/>
-      <c r="K7" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="21">
-        <v>11</v>
-      </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="88"/>
-      <c r="K8" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="21">
-        <v>12</v>
-      </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="88"/>
-      <c r="K9" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <v>13</v>
-      </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="90"/>
-      <c r="K10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="102" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="103"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="104" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="105"/>
-      <c r="H13" s="102" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
-      <c r="K13" s="103"/>
-      <c r="L13" s="106"/>
-      <c r="M13" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="N13" s="73"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="75" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="77" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="79" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="81" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="83" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="75" t="s">
-        <v>43</v>
-      </c>
-      <c r="K14" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="M14" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="N14" s="82" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="74"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="79"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="27">
-        <f>SUM(C16:D16)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="24">
-        <v>0</v>
-      </c>
-      <c r="D16" s="24">
-        <v>0</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="27">
-        <f>SUM(J16:K16)</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="24">
-        <v>0</v>
-      </c>
-      <c r="K16" s="28">
-        <v>0</v>
-      </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N16" s="30">
-        <f>C16</f>
-        <v>0</v>
-      </c>
-    </row>
+    </row>
+    <row r="11" spans="2:24" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="109">
+        <v>14</v>
+      </c>
+      <c r="C11" s="112"/>
+      <c r="D11" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="42">
+        <v>44653.5</v>
+      </c>
+      <c r="G11" s="42">
+        <v>44653.5</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="25">
+    <mergeCell ref="W7:X7"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B3:I3"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="W8:W9"/>
   </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 1 cyclomatic complexity to the code and added the missing rows in the CFG report
</commit_message>
<xml_diff>
--- a/docs/lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/docs/lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D319871F-FFB5-4CF3-87C4-1CE0EB529451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A63C24-6295-4868-A5B5-6C816C1592D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="128">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -453,27 +453,9 @@
     <t>Popa Cosmin-Mihai</t>
   </si>
   <si>
-    <t>9 - 7 + 2 = 4</t>
-  </si>
-  <si>
-    <t>3 + 1 = 4</t>
-  </si>
-  <si>
-    <t>1 - 2(F) - 7</t>
-  </si>
-  <si>
-    <t>1 - 2(T) - 3(F) - 7</t>
-  </si>
-  <si>
-    <t>1 - 2(T) - 3(T) - 4 - 5(F) - 3(F) - 7</t>
-  </si>
-  <si>
     <t>F02_P04</t>
   </si>
   <si>
-    <t>1 - 2(T) - 3(T) - 4 - 5(T) - 3(F) - 7</t>
-  </si>
-  <si>
     <t>tasks, start, end</t>
   </si>
   <si>
@@ -486,12 +468,6 @@
     <t>(3C) i &lt; tasks.length</t>
   </si>
   <si>
-    <t>(5C) nextTime.equals(end)</t>
-  </si>
-  <si>
-    <t>(5C) nextTime.before(end)</t>
-  </si>
-  <si>
     <t>tasks = [...], start = 02/04/2022 12:00, end = 01/04/2022 12:00</t>
   </si>
   <si>
@@ -507,9 +483,6 @@
     <t>tasks = [task activ, repetitiv cu start=04/04/2022 12:00], start = 02/04/2022 12:00, end = 04/04/2022 12:00</t>
   </si>
   <si>
-    <t>tasks = [task activ, repetitiv cu start=03/04/2022 12:00], start = 02/04/2022 12:00, end = 04/04/2022 12:00</t>
-  </si>
-  <si>
     <t>F02_TC03</t>
   </si>
   <si>
@@ -528,28 +501,10 @@
     <t>[task]</t>
   </si>
   <si>
-    <t>1, 2, 7</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>(5C) nextTime!=null &amp;&amp; (nextTime.before(end) || nextTime.equals(end))</t>
-  </si>
-  <si>
     <t>(5C) nextTime!=null</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 7</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 4, 5, 3, 7</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 4, 5, 6, 3, 7</t>
-  </si>
-  <si>
-    <t>1, 2,3 ,4 ,5 ,6, 3, 7</t>
   </si>
   <si>
     <r>
@@ -594,10 +549,61 @@
     <t>[task activ, repetitiv cu start=04/04/2022 12:00]</t>
   </si>
   <si>
-    <t>tasks = [task activ, repetitiv cu start=03/04/2022 12:00]</t>
-  </si>
-  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>4 + 1 = 5</t>
+  </si>
+  <si>
+    <t>F02_P05</t>
+  </si>
+  <si>
+    <t>1 - 2(F) - 8</t>
+  </si>
+  <si>
+    <t>1 - 2(T) - 3(F) - 8</t>
+  </si>
+  <si>
+    <t>1 - 2(T) - 3(T) - 4 - 5(F) - 3(F) - 8</t>
+  </si>
+  <si>
+    <t>1 - 2(T) - 3(T) - 4 - 5(T) - 6(F) - 3(F) - 8</t>
+  </si>
+  <si>
+    <t>1 - 2(T) - 3(T) - 4 - 5(T) - 6(T) - 7 - 3(F) - 8</t>
+  </si>
+  <si>
+    <t>1, 2, 8</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 8</t>
+  </si>
+  <si>
+    <t>11 - 8 + 2 = 5</t>
+  </si>
+  <si>
+    <t>(6C) nextTime.before(end)</t>
+  </si>
+  <si>
+    <t>(6C) nextTime.equals(end)</t>
+  </si>
+  <si>
+    <t>(6C) (nextTime.before(end) || nextTime.equals(end))</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, repetitiv cu start=03/04/2022 12:00, task activ, repetitiv cu start=03/04/2022 12:00], start = 02/04/2022 12:00, end = 04/04/2022 12:00</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 8</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 8</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, repetitiv cu start=03/04/2022 12:00, task activ, repetitiv cu start=03/04/2022 12:00]</t>
+  </si>
+  <si>
+    <t>[task, task]</t>
   </si>
 </sst>
 </file>
@@ -1506,6 +1512,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1518,51 +1533,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1572,25 +1602,55 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1608,9 +1668,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1660,57 +1717,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1734,23 +1740,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>564173</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>388328</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>183173</xdr:rowOff>
+      <xdr:rowOff>153865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>162350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>43962</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>156528</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B0159A9-F992-8ADF-4B8D-5477C0EF21E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8D2D811-F13D-DC27-7C56-4BCE11A06D4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1766,8 +1772,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="564173" y="1326173"/>
-          <a:ext cx="3663462" cy="3027177"/>
+          <a:off x="4615963" y="1296865"/>
+          <a:ext cx="4403480" cy="4003163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1778,23 +1784,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>111687</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>527541</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>124558</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>7328</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142817</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>520211</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>145409</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C80AF29-1A49-EC07-244B-8FC8BE043D9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C1D8B60-8E83-5514-92A2-EEF0C174A3E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1810,8 +1816,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4821117" y="1635687"/>
-          <a:ext cx="4161692" cy="3460130"/>
+          <a:off x="527541" y="1267558"/>
+          <a:ext cx="3626824" cy="3068851"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2127,12 +2133,12 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="33" t="s">
@@ -2261,368 +2267,380 @@
   </sheetPr>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="20" max="20" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="52"/>
+      <c r="B3" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="Q6" s="44" t="s">
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="Q6" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="I8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="49" t="s">
+      <c r="Q8" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
+      <c r="R8" s="64"/>
+      <c r="S8" s="64"/>
       <c r="T8" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
       <c r="I9" s="32"/>
-      <c r="Q9" s="49" t="s">
+      <c r="Q9" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
       <c r="T9" s="28" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="55"/>
-      <c r="Q10" s="49" t="s">
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="57"/>
+      <c r="Q10" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="R10" s="49" t="s">
+      <c r="R10" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="49"/>
+      <c r="S10" s="64"/>
       <c r="T10" s="28" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="60"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="58"/>
-      <c r="Q13" s="44" t="s">
+      <c r="I13" s="58"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="60"/>
+      <c r="Q13" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="60"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I15" s="56"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="60"/>
       <c r="Q15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="62" t="s">
+      <c r="R15" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="62"/>
-      <c r="T15" s="62"/>
+      <c r="S15" s="65"/>
+      <c r="T15" s="65"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I16" s="56"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="60"/>
       <c r="Q16" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="R16" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
+      <c r="R16" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="S16" s="50"/>
+      <c r="T16" s="50"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I17" s="56"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="60"/>
       <c r="Q17" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="R17" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="S17" s="47"/>
-      <c r="T17" s="47"/>
+      <c r="R17" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I18" s="56"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="60"/>
       <c r="Q18" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="R18" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="S18" s="47"/>
-      <c r="T18" s="47"/>
+      <c r="R18" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="e">
         <f>- R19</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I19" s="56"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="60"/>
       <c r="Q19" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="R19" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="S19" s="47"/>
-      <c r="T19" s="47"/>
+        <v>83</v>
+      </c>
+      <c r="R19" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I20" s="56"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="58"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="47"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="47"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="60"/>
+      <c r="Q20" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="R20" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="56"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="60"/>
       <c r="Q21" s="29"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="56"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57"/>
-      <c r="O22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="60"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I23" s="56"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="60"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I24" s="59"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2639,14 +2657,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2659,10 +2669,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:AB16"/>
+  <dimension ref="B1:AC16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,179 +2689,184 @@
     <col min="16" max="16" width="10.85546875" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" customWidth="1"/>
     <col min="18" max="19" width="8.85546875" customWidth="1"/>
-    <col min="22" max="24" width="8.5703125" customWidth="1"/>
-    <col min="25" max="25" width="8.7109375" customWidth="1"/>
-    <col min="26" max="27" width="8.5703125" customWidth="1"/>
-    <col min="28" max="28" width="8.42578125" customWidth="1"/>
+    <col min="23" max="25" width="8.5703125" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" customWidth="1"/>
+    <col min="27" max="28" width="8.5703125" customWidth="1"/>
+    <col min="29" max="29" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B3" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52"/>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B3" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="70" t="s">
+    <row r="6" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
-      <c r="X6" s="70"/>
-      <c r="Y6" s="70"/>
-      <c r="Z6" s="70"/>
-      <c r="AA6" s="70"/>
-      <c r="AB6" s="70"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="66" t="s">
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="67"/>
+      <c r="Z6" s="67"/>
+      <c r="AA6" s="67"/>
+      <c r="AB6" s="67"/>
+      <c r="AC6" s="67"/>
+    </row>
+    <row r="7" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
-      <c r="O7" s="65"/>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="65"/>
-      <c r="R7" s="67" t="s">
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="68" t="s">
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="68"/>
-      <c r="X7" s="68"/>
-      <c r="Y7" s="68"/>
-      <c r="Z7" s="68"/>
-      <c r="AA7" s="68"/>
-      <c r="AB7" s="68"/>
-    </row>
-    <row r="8" spans="2:28" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="70"/>
-      <c r="C8" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="66"/>
-      <c r="F8" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65" t="s">
+      <c r="X7" s="70"/>
+      <c r="Y7" s="70"/>
+      <c r="Z7" s="70"/>
+      <c r="AA7" s="70"/>
+      <c r="AB7" s="70"/>
+      <c r="AC7" s="70"/>
+    </row>
+    <row r="8" spans="2:29" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="67"/>
+      <c r="C8" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="75"/>
+      <c r="F8" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="S8" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="U8" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="V8" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="S8" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="T8" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="U8" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="V8" s="68">
+      <c r="W8" s="70">
         <v>0</v>
       </c>
-      <c r="W8" s="68">
+      <c r="X8" s="70">
         <v>1</v>
       </c>
-      <c r="X8" s="68">
+      <c r="Y8" s="70">
         <v>2</v>
       </c>
-      <c r="Y8" s="68" t="s">
+      <c r="Z8" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="Z8" s="68" t="s">
+      <c r="AA8" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="AA8" s="68" t="s">
+      <c r="AB8" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AB8" s="68" t="s">
+      <c r="AC8" s="70" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="70"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="66"/>
+    <row r="9" spans="2:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="67"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="75"/>
       <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
@@ -2888,34 +2903,35 @@
       <c r="Q9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="67"/>
-      <c r="S9" s="67"/>
-      <c r="T9" s="67"/>
-      <c r="U9" s="67"/>
-      <c r="V9" s="68"/>
-      <c r="W9" s="68"/>
-      <c r="X9" s="68"/>
-      <c r="Y9" s="68"/>
-      <c r="Z9" s="68"/>
-      <c r="AA9" s="68"/>
-      <c r="AB9" s="68"/>
-    </row>
-    <row r="10" spans="2:28" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
+      <c r="Y9" s="70"/>
+      <c r="Z9" s="70"/>
+      <c r="AA9" s="70"/>
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="70"/>
+    </row>
+    <row r="10" spans="2:29" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2928,41 +2944,42 @@
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
       <c r="R10" s="15" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
-      <c r="V10" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="W10" s="16"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
       <c r="AA10" s="16"/>
       <c r="AB10" s="16"/>
-    </row>
-    <row r="11" spans="2:28" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC10" s="16"/>
+    </row>
+    <row r="11" spans="2:29" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="E11" s="13" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -2974,262 +2991,282 @@
       <c r="Q11" s="14"/>
       <c r="R11" s="15"/>
       <c r="S11" s="15" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
-      <c r="V11" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="W11" s="16"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="X11" s="16"/>
       <c r="Y11" s="16"/>
       <c r="Z11" s="16"/>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
-    </row>
-    <row r="12" spans="2:28" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC11" s="16"/>
+    </row>
+    <row r="12" spans="2:29" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="I12" s="14"/>
+        <v>99</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="J12" s="14"/>
       <c r="K12" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="14" t="s">
-        <v>109</v>
-      </c>
+      <c r="Q12" s="14"/>
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
       <c r="T12" s="15" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="U12" s="15"/>
-      <c r="V12" s="16"/>
+      <c r="V12" s="15"/>
       <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
+      <c r="X12" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="Y12" s="16"/>
-      <c r="Z12" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="AB12" s="16"/>
-    </row>
-    <row r="13" spans="2:28" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC12" s="16"/>
+    </row>
+    <row r="13" spans="2:29" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="14"/>
+        <v>99</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="J13" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
-      <c r="T13" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="U13" s="15"/>
-      <c r="V13" s="16"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="V13" s="15"/>
       <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
+      <c r="X13" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="Y13" s="16"/>
-      <c r="Z13" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA13" s="16"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="AB13" s="16"/>
-    </row>
-    <row r="14" spans="2:28" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC13" s="16"/>
+    </row>
+    <row r="14" spans="2:29" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="I14" s="14"/>
+        <v>99</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="J14" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="O14" s="14"/>
       <c r="P14" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
-      <c r="U14" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="V14" s="16"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15" t="s">
+        <v>99</v>
+      </c>
       <c r="W14" s="16"/>
-      <c r="X14" s="16"/>
+      <c r="X14" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="Y14" s="16"/>
-      <c r="Z14" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="AB14" s="16"/>
-    </row>
-    <row r="15" spans="2:28" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC14" s="16"/>
+    </row>
+    <row r="15" spans="2:29" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="I15" s="14"/>
+        <v>99</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="J15" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="Q15" s="14"/>
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
-      <c r="U15" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="V15" s="16"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15" t="s">
+        <v>99</v>
+      </c>
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA15" s="16"/>
+      <c r="Y15" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="AB15" s="16"/>
-    </row>
-    <row r="16" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AC15" s="16"/>
+    </row>
+    <row r="16" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:AB6"/>
-    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="E6:AC6"/>
     <mergeCell ref="AA8:AA9"/>
+    <mergeCell ref="AB8:AB9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="W8:W9"/>
     <mergeCell ref="X8:X9"/>
     <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="V7:AB7"/>
-    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="W7:AC7"/>
+    <mergeCell ref="AC8:AC9"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:Q7"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3243,8 +3280,8 @@
   </sheetPr>
   <dimension ref="B1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3262,57 +3299,57 @@
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="101" t="s">
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="102"/>
+      <c r="I4" s="82"/>
     </row>
     <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="100"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="106"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="87"/>
       <c r="E5" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
@@ -3322,17 +3359,17 @@
       </c>
     </row>
     <row r="6" spans="2:24" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="107">
+      <c r="B6" s="44">
         <v>9</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="88" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="37" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="F6" s="38">
         <v>44653.5</v>
@@ -3341,10 +3378,10 @@
         <v>44652.5</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>10</v>
@@ -3352,15 +3389,15 @@
       <c r="U6" s="18"/>
     </row>
     <row r="7" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="108">
+      <c r="B7" s="45">
         <v>10</v>
       </c>
-      <c r="C7" s="111"/>
+      <c r="C7" s="89"/>
       <c r="D7" s="39" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F7" s="40">
         <v>44653.5</v>
@@ -3369,43 +3406,43 @@
         <v>44654.5</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="L7" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="75" t="s">
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="73" t="s">
+      <c r="Q7" s="94"/>
+      <c r="R7" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="92"/>
-      <c r="W7" s="96" t="s">
+      <c r="S7" s="92"/>
+      <c r="T7" s="92"/>
+      <c r="U7" s="92"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="X7" s="97"/>
+      <c r="X7" s="77"/>
     </row>
     <row r="8" spans="2:24" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="108">
+      <c r="B8" s="45">
         <v>11</v>
       </c>
-      <c r="C8" s="111"/>
+      <c r="C8" s="89"/>
       <c r="D8" s="39" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="F8" s="40">
         <v>44653.5</v>
@@ -3414,61 +3451,61 @@
         <v>44654.5</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I8" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="L8" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="83" t="s">
+      <c r="M8" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="83" t="s">
+      <c r="N8" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="89" t="s">
+      <c r="O8" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="P8" s="79" t="s">
+      <c r="P8" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="Q8" s="77" t="s">
+      <c r="Q8" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="R8" s="80" t="s">
+      <c r="R8" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="S8" s="82" t="s">
+      <c r="S8" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="T8" s="82" t="s">
+      <c r="T8" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="84" t="s">
+      <c r="U8" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="V8" s="93" t="s">
+      <c r="V8" s="110" t="s">
         <v>74</v>
       </c>
-      <c r="W8" s="95" t="s">
+      <c r="W8" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="X8" s="78" t="s">
+      <c r="X8" s="84" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="108">
+      <c r="B9" s="45">
         <v>12</v>
       </c>
-      <c r="C9" s="111"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="39" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="F9" s="40">
         <v>44653.5</v>
@@ -3477,35 +3514,35 @@
         <v>44654.5</v>
       </c>
       <c r="H9" s="39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="L9" s="87"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="88"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="77"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="83"/>
-      <c r="T9" s="83"/>
-      <c r="U9" s="85"/>
-      <c r="V9" s="94"/>
-      <c r="W9" s="86"/>
-      <c r="X9" s="79"/>
+        <v>97</v>
+      </c>
+      <c r="L9" s="104"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="107"/>
+      <c r="P9" s="108"/>
+      <c r="Q9" s="95"/>
+      <c r="R9" s="98"/>
+      <c r="S9" s="100"/>
+      <c r="T9" s="100"/>
+      <c r="U9" s="102"/>
+      <c r="V9" s="111"/>
+      <c r="W9" s="103"/>
+      <c r="X9" s="96"/>
     </row>
     <row r="10" spans="2:24" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="108">
+      <c r="B10" s="45">
         <v>13</v>
       </c>
-      <c r="C10" s="111"/>
+      <c r="C10" s="89"/>
       <c r="D10" s="39" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="F10" s="40">
         <v>44653.5</v>
@@ -3514,10 +3551,10 @@
         <v>44655.5</v>
       </c>
       <c r="H10" s="39" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I10" s="39" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="L10" s="21">
         <f>SUM(M10:N10)</f>
@@ -3530,7 +3567,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="43" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="P10" s="20">
         <v>0</v>
@@ -3560,16 +3597,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:24" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="109">
+    <row r="11" spans="2:24" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="46">
         <v>14</v>
       </c>
-      <c r="C11" s="112"/>
+      <c r="C11" s="90"/>
       <c r="D11" s="41" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F11" s="42">
         <v>44653.5</v>
@@ -3578,15 +3615,24 @@
         <v>44653.5</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="I11" s="41" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
     <mergeCell ref="W7:X7"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:I3"/>
@@ -3603,15 +3649,6 @@
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="U8:U9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="W8:W9"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3620,12 +3657,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3773,15 +3807,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3805,10 +3843,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added code coverage report
</commit_message>
<xml_diff>
--- a/docs/lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/docs/lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A63C24-6295-4868-A5B5-6C816C1592D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10371FA-88BC-459E-A50A-890E5D2DC9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -547,9 +547,6 @@
   </si>
   <si>
     <t>[task activ, repetitiv cu start=04/04/2022 12:00]</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>4 + 1 = 5</t>
@@ -1461,7 +1458,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1533,6 +1529,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1542,9 +1544,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1572,12 +1571,27 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1590,22 +1604,49 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1653,12 +1694,6 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1668,57 +1703,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2133,15 +2130,15 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2159,11 +2156,11 @@
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="29" t="s">
+      <c r="N5" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -2233,7 +2230,7 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="1"/>
@@ -2267,7 +2264,7 @@
   </sheetPr>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
@@ -2280,109 +2277,109 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="49"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="54"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="I6" s="47" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="I6" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="Q6" s="47" t="s">
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="Q6" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
       <c r="I8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="64" t="s">
+      <c r="Q8" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="28">
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="27">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="I9" s="32"/>
-      <c r="Q9" s="64" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="I9" s="31"/>
+      <c r="Q9" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="28" t="s">
-        <v>119</v>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="27" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
       <c r="I10" s="55" t="s">
         <v>33</v>
       </c>
@@ -2392,28 +2389,28 @@
       <c r="M10" s="56"/>
       <c r="N10" s="56"/>
       <c r="O10" s="57"/>
-      <c r="Q10" s="64" t="s">
+      <c r="Q10" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="R10" s="64" t="s">
+      <c r="R10" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="64"/>
-      <c r="T10" s="28" t="s">
-        <v>110</v>
+      <c r="S10" s="51"/>
+      <c r="T10" s="27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
       <c r="I11" s="58"/>
       <c r="J11" s="59"/>
       <c r="K11" s="59"/>
@@ -2423,16 +2420,16 @@
       <c r="O11" s="60"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
       <c r="I12" s="58"/>
       <c r="J12" s="59"/>
       <c r="K12" s="59"/>
@@ -2442,16 +2439,16 @@
       <c r="O12" s="60"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="I13" s="58"/>
       <c r="J13" s="59"/>
       <c r="K13" s="59"/>
@@ -2459,24 +2456,24 @@
       <c r="M13" s="59"/>
       <c r="N13" s="59"/>
       <c r="O13" s="60"/>
-      <c r="Q13" s="47" t="s">
+      <c r="Q13" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
       <c r="I14" s="58"/>
       <c r="J14" s="59"/>
       <c r="K14" s="59"/>
@@ -2493,14 +2490,14 @@
       <c r="M15" s="59"/>
       <c r="N15" s="59"/>
       <c r="O15" s="60"/>
-      <c r="Q15" s="26" t="s">
+      <c r="Q15" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="65" t="s">
+      <c r="R15" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="65"/>
-      <c r="T15" s="65"/>
+      <c r="S15" s="64"/>
+      <c r="T15" s="64"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I16" s="58"/>
@@ -2510,14 +2507,14 @@
       <c r="M16" s="59"/>
       <c r="N16" s="59"/>
       <c r="O16" s="60"/>
-      <c r="Q16" s="29" t="s">
+      <c r="Q16" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="R16" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
+      <c r="R16" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I17" s="58"/>
@@ -2527,14 +2524,14 @@
       <c r="M17" s="59"/>
       <c r="N17" s="59"/>
       <c r="O17" s="60"/>
-      <c r="Q17" s="29" t="s">
+      <c r="Q17" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="R17" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="S17" s="50"/>
-      <c r="T17" s="50"/>
+      <c r="R17" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I18" s="58"/>
@@ -2544,14 +2541,14 @@
       <c r="M18" s="59"/>
       <c r="N18" s="59"/>
       <c r="O18" s="60"/>
-      <c r="Q18" s="29" t="s">
+      <c r="Q18" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="R18" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="S18" s="50"/>
-      <c r="T18" s="50"/>
+      <c r="R18" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="e">
@@ -2565,14 +2562,14 @@
       <c r="M19" s="59"/>
       <c r="N19" s="59"/>
       <c r="O19" s="60"/>
-      <c r="Q19" s="29" t="s">
+      <c r="Q19" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="R19" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="S19" s="50"/>
-      <c r="T19" s="50"/>
+      <c r="R19" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I20" s="58"/>
@@ -2582,14 +2579,14 @@
       <c r="M20" s="59"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
-      <c r="Q20" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="R20" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="S20" s="50"/>
-      <c r="T20" s="50"/>
+      <c r="Q20" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="R20" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I21" s="58"/>
@@ -2599,10 +2596,10 @@
       <c r="M21" s="59"/>
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="50"/>
-      <c r="T21" s="50"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I22" s="58"/>
@@ -2633,14 +2630,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2657,6 +2646,14 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2697,91 +2694,91 @@
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
-      <c r="Y6" s="67"/>
-      <c r="Z6" s="67"/>
-      <c r="AA6" s="67"/>
-      <c r="AB6" s="67"/>
-      <c r="AC6" s="67"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="72"/>
+      <c r="U6" s="72"/>
+      <c r="V6" s="72"/>
+      <c r="W6" s="72"/>
+      <c r="X6" s="72"/>
+      <c r="Y6" s="72"/>
+      <c r="Z6" s="72"/>
+      <c r="AA6" s="72"/>
+      <c r="AB6" s="72"/>
+      <c r="AC6" s="72"/>
     </row>
     <row r="7" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="75" t="s">
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="74" t="s">
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="74"/>
+      <c r="S7" s="69"/>
+      <c r="T7" s="69"/>
+      <c r="U7" s="69"/>
+      <c r="V7" s="69"/>
       <c r="W7" s="70" t="s">
         <v>20</v>
       </c>
@@ -2793,52 +2790,52 @@
       <c r="AC7" s="70"/>
     </row>
     <row r="8" spans="2:29" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="67"/>
-      <c r="C8" s="71" t="s">
+      <c r="B8" s="72"/>
+      <c r="C8" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="73" t="s">
+      <c r="E8" s="68"/>
+      <c r="F8" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73" t="s">
+      <c r="G8" s="67"/>
+      <c r="H8" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73" t="s">
+      <c r="I8" s="67"/>
+      <c r="J8" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73" t="s">
+      <c r="K8" s="67"/>
+      <c r="L8" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73" t="s">
+      <c r="O8" s="67"/>
+      <c r="P8" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="73"/>
-      <c r="P8" s="73" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="74" t="s">
+      <c r="Q8" s="67"/>
+      <c r="R8" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="S8" s="74" t="s">
+      <c r="S8" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="74" t="s">
+      <c r="T8" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="U8" s="74" t="s">
+      <c r="U8" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="V8" s="74" t="s">
-        <v>111</v>
+      <c r="V8" s="69" t="s">
+        <v>110</v>
       </c>
       <c r="W8" s="70">
         <v>0</v>
@@ -2863,10 +2860,10 @@
       </c>
     </row>
     <row r="9" spans="2:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="67"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="75"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
@@ -2903,11 +2900,11 @@
       <c r="Q9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="74"/>
-      <c r="S9" s="74"/>
-      <c r="T9" s="74"/>
-      <c r="U9" s="74"/>
-      <c r="V9" s="74"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
       <c r="W9" s="70"/>
       <c r="X9" s="70"/>
       <c r="Y9" s="70"/>
@@ -2920,14 +2917,14 @@
       <c r="B10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="33" t="s">
         <v>88</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14" t="s">
@@ -2964,14 +2961,14 @@
       <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="34" t="s">
         <v>89</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>99</v>
@@ -3010,14 +3007,14 @@
       <c r="B12" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="35" t="s">
         <v>97</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>99</v>
@@ -3062,14 +3059,14 @@
       <c r="B13" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>91</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>99</v>
@@ -3120,14 +3117,14 @@
       <c r="B14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>92</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>98</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>99</v>
@@ -3178,14 +3175,14 @@
       <c r="B15" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="35" t="s">
-        <v>123</v>
+      <c r="C15" s="34" t="s">
+        <v>122</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>98</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>99</v>
@@ -3237,20 +3234,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:Q7"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="W8:W9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -3267,6 +3250,20 @@
     <mergeCell ref="W7:AC7"/>
     <mergeCell ref="AC8:AC9"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="V8:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3280,8 +3277,8 @@
   </sheetPr>
   <dimension ref="B1:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3299,49 +3296,49 @@
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="81" t="s">
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="82"/>
+      <c r="I4" s="96"/>
     </row>
     <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="80"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="87"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="101"/>
       <c r="E5" s="2" t="s">
         <v>103</v>
       </c>
@@ -3359,28 +3356,28 @@
       </c>
     </row>
     <row r="6" spans="2:24" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="44">
+      <c r="B6" s="43">
         <v>9</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="37">
         <v>44653.5</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="37">
         <v>44652.5</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="36" t="s">
         <v>97</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -3389,171 +3386,171 @@
       <c r="U6" s="18"/>
     </row>
     <row r="7" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="45">
+      <c r="B7" s="44">
         <v>10</v>
       </c>
-      <c r="C7" s="89"/>
-      <c r="D7" s="39" t="s">
+      <c r="C7" s="103"/>
+      <c r="D7" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="39">
         <v>44653.5</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="39">
         <v>44654.5</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="I7" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="91" t="s">
+      <c r="L7" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="92"/>
-      <c r="P7" s="93" t="s">
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="91" t="s">
+      <c r="Q7" s="106"/>
+      <c r="R7" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="S7" s="92"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="92"/>
-      <c r="V7" s="109"/>
-      <c r="W7" s="76" t="s">
+      <c r="S7" s="78"/>
+      <c r="T7" s="78"/>
+      <c r="U7" s="78"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="X7" s="77"/>
+      <c r="X7" s="91"/>
     </row>
     <row r="8" spans="2:24" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <v>11</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="103"/>
+      <c r="D8" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="39">
         <v>44653.5</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="39">
         <v>44654.5</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="L8" s="103" t="s">
+      <c r="L8" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="100" t="s">
+      <c r="M8" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="100" t="s">
+      <c r="N8" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="106" t="s">
+      <c r="O8" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="P8" s="96" t="s">
+      <c r="P8" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="Q8" s="95" t="s">
+      <c r="Q8" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="R8" s="97" t="s">
+      <c r="R8" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="S8" s="99" t="s">
+      <c r="S8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="T8" s="99" t="s">
+      <c r="T8" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="101" t="s">
+      <c r="U8" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="V8" s="110" t="s">
+      <c r="V8" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="W8" s="112" t="s">
+      <c r="W8" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="X8" s="84" t="s">
+      <c r="X8" s="98" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <v>12</v>
       </c>
-      <c r="C9" s="89"/>
-      <c r="D9" s="39" t="s">
+      <c r="C9" s="103"/>
+      <c r="D9" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="39">
         <v>44653.5</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="39">
         <v>44654.5</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="L9" s="104"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="107"/>
-      <c r="P9" s="108"/>
-      <c r="Q9" s="95"/>
-      <c r="R9" s="98"/>
-      <c r="S9" s="100"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="102"/>
-      <c r="V9" s="111"/>
-      <c r="W9" s="103"/>
-      <c r="X9" s="96"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="89"/>
+      <c r="Q9" s="107"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="76"/>
+      <c r="T9" s="76"/>
+      <c r="U9" s="111"/>
+      <c r="V9" s="81"/>
+      <c r="W9" s="83"/>
+      <c r="X9" s="88"/>
     </row>
     <row r="10" spans="2:24" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="45">
+      <c r="B10" s="44">
         <v>13</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="39" t="s">
+      <c r="C10" s="103"/>
+      <c r="D10" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="39">
         <v>44653.5</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="39">
         <v>44655.5</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="39" t="s">
+      <c r="I10" s="38" t="s">
         <v>98</v>
       </c>
       <c r="L10" s="21">
@@ -3566,8 +3563,8 @@
       <c r="N10" s="19">
         <v>0</v>
       </c>
-      <c r="O10" s="43" t="s">
-        <v>109</v>
+      <c r="O10" s="42">
+        <v>1</v>
       </c>
       <c r="P10" s="20">
         <v>0</v>
@@ -3588,42 +3585,59 @@
       <c r="U10" s="22">
         <v>0</v>
       </c>
-      <c r="V10" s="23"/>
+      <c r="V10" s="112">
+        <v>1</v>
+      </c>
       <c r="W10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="X10" s="24">
+      <c r="X10" s="23">
         <f>M10</f>
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:24" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>14</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="41" t="s">
+      <c r="C11" s="104"/>
+      <c r="D11" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="41">
+        <v>44653.5</v>
+      </c>
+      <c r="G11" s="41">
+        <v>44653.5</v>
+      </c>
+      <c r="H11" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="F11" s="42">
-        <v>44653.5</v>
-      </c>
-      <c r="G11" s="42">
-        <v>44653.5</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="41" t="s">
-        <v>127</v>
+      <c r="I11" s="40" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="R7:V7"/>
     <mergeCell ref="V8:V9"/>
@@ -3634,21 +3648,6 @@
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
     <mergeCell ref="W7:X7"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="X8:X9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="U8:U9"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3657,9 +3656,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3807,19 +3809,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3843,9 +3841,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated dates in WBT spreadsheets
</commit_message>
<xml_diff>
--- a/docs/lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/docs/lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10371FA-88BC-459E-A50A-890E5D2DC9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462F0F99-0609-492E-9012-71052B99F07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -468,21 +468,6 @@
     <t>(3C) i &lt; tasks.length</t>
   </si>
   <si>
-    <t>tasks = [...], start = 02/04/2022 12:00, end = 01/04/2022 12:00</t>
-  </si>
-  <si>
-    <t>tasks = [], start = 02/04/2022 12:00, end = 03/04/2022 12:00</t>
-  </si>
-  <si>
-    <t>tasks = [task activ, nerepetitiv cu start=03/04/2022 12:00], start = 02/04/2022 12:00, end = 03/04/2022 12:00</t>
-  </si>
-  <si>
-    <t>tasks = [task activ, repetitiv cu start=04/04/2022 12:00], start = 02/04/2022 12:00, end = 03/04/2022 12:00</t>
-  </si>
-  <si>
-    <t>tasks = [task activ, repetitiv cu start=04/04/2022 12:00], start = 02/04/2022 12:00, end = 04/04/2022 12:00</t>
-  </si>
-  <si>
     <t>F02_TC03</t>
   </si>
   <si>
@@ -540,15 +525,6 @@
     <t>end</t>
   </si>
   <si>
-    <t>[[task activ, nerepetitiv cu start=03/04/2022 12:00]]</t>
-  </si>
-  <si>
-    <t>[task activ, nerepetitiv cu start=03/04/2022 12:00]</t>
-  </si>
-  <si>
-    <t>[task activ, repetitiv cu start=04/04/2022 12:00]</t>
-  </si>
-  <si>
     <t>4 + 1 = 5</t>
   </si>
   <si>
@@ -588,19 +564,43 @@
     <t>(6C) (nextTime.before(end) || nextTime.equals(end))</t>
   </si>
   <si>
-    <t>tasks = [task activ, repetitiv cu start=03/04/2022 12:00, task activ, repetitiv cu start=03/04/2022 12:00], start = 02/04/2022 12:00, end = 04/04/2022 12:00</t>
-  </si>
-  <si>
     <t>1, 2, 3, 4, 5, 6, 8</t>
   </si>
   <si>
     <t>1, 2, 3, 4, 5, 8</t>
   </si>
   <si>
-    <t>tasks = [task activ, repetitiv cu start=03/04/2022 12:00, task activ, repetitiv cu start=03/04/2022 12:00]</t>
-  </si>
-  <si>
     <t>[task, task]</t>
+  </si>
+  <si>
+    <t>[[task activ, nerepetitiv cu start=03/04/2024 12:00]]</t>
+  </si>
+  <si>
+    <t>[task activ, nerepetitiv cu start=03/04/2024 12:00]</t>
+  </si>
+  <si>
+    <t>[task activ, repetitiv cu start=04/04/2024 12:00]</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, repetitiv cu start=03/04/2024 12:00, task activ, repetitiv cu start=03/04/2024 12:00]</t>
+  </si>
+  <si>
+    <t>tasks = [...], start = 02/04/2024 12:00, end = 01/04/2024 12:00</t>
+  </si>
+  <si>
+    <t>tasks = [], start = 02/04/2024 12:00, end = 03/04/2024 12:00</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, nerepetitiv cu start=03/04/2024 12:00], start = 02/04/2024 12:00, end = 03/04/2024 12:00</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, repetitiv cu start=04/04/2024 12:00], start = 02/04/2024 12:00, end = 03/04/2024 12:00</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, repetitiv cu start=04/04/2024 12:00], start = 02/04/2024 12:00, end = 04/04/2024 12:00</t>
+  </si>
+  <si>
+    <t>tasks = [task activ, repetitiv cu start=03/04/2024 12:00, task activ, repetitiv cu start=03/04/2024 12:00], start = 02/04/2024 12:00, end = 04/04/2024 12:00</t>
   </si>
 </sst>
 </file>
@@ -1517,6 +1517,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1529,51 +1530,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1583,31 +1599,19 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1616,6 +1620,66 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1643,9 +1707,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1655,67 +1716,6 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2130,12 +2130,12 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="s">
@@ -2277,73 +2277,73 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="B3" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="Q6" s="46" t="s">
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="Q6" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="I8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="51" t="s">
+      <c r="Q8" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
+      <c r="R8" s="64"/>
+      <c r="S8" s="64"/>
       <c r="T8" s="27">
         <v>5</v>
       </c>
@@ -2352,32 +2352,32 @@
       <c r="B9" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="I9" s="31"/>
-      <c r="Q9" s="51" t="s">
+      <c r="Q9" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
       <c r="T9" s="27" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="I10" s="55" t="s">
@@ -2389,26 +2389,26 @@
       <c r="M10" s="56"/>
       <c r="N10" s="56"/>
       <c r="O10" s="57"/>
-      <c r="Q10" s="51" t="s">
+      <c r="Q10" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="R10" s="51" t="s">
+      <c r="R10" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="51"/>
+      <c r="S10" s="64"/>
       <c r="T10" s="27" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="I11" s="58"/>
@@ -2423,11 +2423,11 @@
       <c r="B12" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="I12" s="58"/>
@@ -2442,11 +2442,11 @@
       <c r="B13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="I13" s="58"/>
@@ -2456,22 +2456,22 @@
       <c r="M13" s="59"/>
       <c r="N13" s="59"/>
       <c r="O13" s="60"/>
-      <c r="Q13" s="46" t="s">
+      <c r="Q13" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="R13" s="47"/>
-      <c r="S13" s="47"/>
-      <c r="T13" s="47"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="I14" s="58"/>
@@ -2493,11 +2493,11 @@
       <c r="Q15" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="64" t="s">
+      <c r="R15" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="64"/>
-      <c r="T15" s="64"/>
+      <c r="S15" s="65"/>
+      <c r="T15" s="65"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I16" s="58"/>
@@ -2510,11 +2510,11 @@
       <c r="Q16" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="R16" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="S16" s="49"/>
-      <c r="T16" s="49"/>
+      <c r="R16" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="S16" s="50"/>
+      <c r="T16" s="50"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I17" s="58"/>
@@ -2527,11 +2527,11 @@
       <c r="Q17" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="R17" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="S17" s="49"/>
-      <c r="T17" s="49"/>
+      <c r="R17" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I18" s="58"/>
@@ -2544,11 +2544,11 @@
       <c r="Q18" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="R18" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
+      <c r="R18" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="e">
@@ -2565,11 +2565,11 @@
       <c r="Q19" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="R19" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="S19" s="49"/>
-      <c r="T19" s="49"/>
+      <c r="R19" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I20" s="58"/>
@@ -2580,13 +2580,13 @@
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
       <c r="Q20" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="R20" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="S20" s="49"/>
-      <c r="T20" s="49"/>
+        <v>102</v>
+      </c>
+      <c r="R20" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I21" s="58"/>
@@ -2597,9 +2597,9 @@
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
       <c r="Q21" s="28"/>
-      <c r="R21" s="49"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I22" s="58"/>
@@ -2630,6 +2630,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2646,14 +2654,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2668,7 +2668,7 @@
   </sheetPr>
   <dimension ref="B1:AC16"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -2694,91 +2694,91 @@
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B3" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="54"/>
+      <c r="B3" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="72"/>
-      <c r="U6" s="72"/>
-      <c r="V6" s="72"/>
-      <c r="W6" s="72"/>
-      <c r="X6" s="72"/>
-      <c r="Y6" s="72"/>
-      <c r="Z6" s="72"/>
-      <c r="AA6" s="72"/>
-      <c r="AB6" s="72"/>
-      <c r="AC6" s="72"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="67"/>
+      <c r="Z6" s="67"/>
+      <c r="AA6" s="67"/>
+      <c r="AB6" s="67"/>
+      <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="68" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="69" t="s">
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
       <c r="W7" s="70" t="s">
         <v>20</v>
       </c>
@@ -2790,52 +2790,52 @@
       <c r="AC7" s="70"/>
     </row>
     <row r="8" spans="2:29" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="72"/>
-      <c r="C8" s="65" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="67" t="s">
+      <c r="E8" s="75"/>
+      <c r="F8" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67" t="s">
+      <c r="G8" s="73"/>
+      <c r="H8" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67" t="s">
-        <v>119</v>
-      </c>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67" t="s">
-        <v>120</v>
-      </c>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="69" t="s">
+      <c r="I8" s="73"/>
+      <c r="J8" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73" t="s">
+        <v>111</v>
+      </c>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="S8" s="69" t="s">
+      <c r="S8" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="69" t="s">
+      <c r="T8" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="U8" s="69" t="s">
+      <c r="U8" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="V8" s="69" t="s">
-        <v>110</v>
+      <c r="V8" s="74" t="s">
+        <v>102</v>
       </c>
       <c r="W8" s="70">
         <v>0</v>
@@ -2860,10 +2860,10 @@
       </c>
     </row>
     <row r="9" spans="2:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="72"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="68"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="75"/>
       <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
@@ -2900,11 +2900,11 @@
       <c r="Q9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="69"/>
-      <c r="V9" s="69"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
       <c r="W9" s="70"/>
       <c r="X9" s="70"/>
       <c r="Y9" s="70"/>
@@ -2918,17 +2918,17 @@
         <v>52</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2941,14 +2941,14 @@
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
       <c r="R10" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
       <c r="V10" s="15"/>
       <c r="W10" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
@@ -2962,21 +2962,21 @@
         <v>53</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -2988,13 +2988,13 @@
       <c r="Q11" s="14"/>
       <c r="R11" s="15"/>
       <c r="S11" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
       <c r="V11" s="15"/>
       <c r="W11" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="X11" s="16"/>
       <c r="Y11" s="16"/>
@@ -3005,30 +3005,30 @@
     </row>
     <row r="12" spans="2:29" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
@@ -3039,117 +3039,117 @@
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
       <c r="T12" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="U12" s="15"/>
       <c r="V12" s="15"/>
       <c r="W12" s="16"/>
       <c r="X12" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
       <c r="AA12" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AB12" s="16"/>
       <c r="AC12" s="16"/>
     </row>
     <row r="13" spans="2:29" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
       <c r="U13" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="V13" s="15"/>
       <c r="W13" s="16"/>
       <c r="X13" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Y13" s="16"/>
       <c r="Z13" s="16"/>
       <c r="AA13" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AB13" s="16"/>
       <c r="AC13" s="16"/>
     </row>
     <row r="14" spans="2:29" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="O14" s="14"/>
       <c r="P14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="15"/>
@@ -3157,57 +3157,57 @@
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
       <c r="V14" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="W14" s="16"/>
       <c r="X14" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Y14" s="16"/>
       <c r="Z14" s="16"/>
       <c r="AA14" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AB14" s="16"/>
       <c r="AC14" s="16"/>
     </row>
     <row r="15" spans="2:29" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Q15" s="14"/>
       <c r="R15" s="15"/>
@@ -3215,16 +3215,16 @@
       <c r="T15" s="15"/>
       <c r="U15" s="15"/>
       <c r="V15" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
       <c r="Y15" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Z15" s="16"/>
       <c r="AA15" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="AB15" s="16"/>
       <c r="AC15" s="16"/>
@@ -3234,6 +3234,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -3250,20 +3264,6 @@
     <mergeCell ref="W7:AC7"/>
     <mergeCell ref="AC8:AC9"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="W8:W9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:Q7"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="V8:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3277,8 +3277,8 @@
   </sheetPr>
   <dimension ref="B1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3296,12 +3296,12 @@
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="92" t="s">
@@ -3319,10 +3319,10 @@
       <c r="B4" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="99" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="95" t="s">
@@ -3337,16 +3337,16 @@
     </row>
     <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="94"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="101"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="100"/>
       <c r="E5" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
@@ -3359,26 +3359,26 @@
       <c r="B6" s="43">
         <v>9</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="76" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="F6" s="37">
-        <v>44653.5</v>
+        <v>45384.5</v>
       </c>
       <c r="G6" s="37">
-        <v>44652.5</v>
+        <v>45383.5</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>10</v>
@@ -3389,107 +3389,107 @@
       <c r="B7" s="44">
         <v>10</v>
       </c>
-      <c r="C7" s="103"/>
+      <c r="C7" s="77"/>
       <c r="D7" s="38" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F7" s="39">
-        <v>44653.5</v>
+        <v>45384.5</v>
       </c>
       <c r="G7" s="39">
-        <v>44654.5</v>
+        <v>45385.5</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="L7" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="105" t="s">
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="77" t="s">
+      <c r="Q7" s="82"/>
+      <c r="R7" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="S7" s="78"/>
-      <c r="T7" s="78"/>
-      <c r="U7" s="78"/>
-      <c r="V7" s="79"/>
-      <c r="W7" s="90" t="s">
+      <c r="S7" s="80"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="101"/>
+      <c r="W7" s="111" t="s">
         <v>69</v>
       </c>
-      <c r="X7" s="91"/>
+      <c r="X7" s="112"/>
     </row>
     <row r="8" spans="2:24" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="44">
         <v>11</v>
       </c>
-      <c r="C8" s="103"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="38" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F8" s="39">
-        <v>44653.5</v>
+        <v>45384.5</v>
       </c>
       <c r="G8" s="39">
-        <v>44654.5</v>
+        <v>45385.5</v>
       </c>
       <c r="H8" s="38" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="L8" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="76" t="s">
+      <c r="M8" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="76" t="s">
+      <c r="N8" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="86" t="s">
+      <c r="O8" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="Q8" s="107" t="s">
+      <c r="Q8" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="R8" s="108" t="s">
+      <c r="R8" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="S8" s="75" t="s">
+      <c r="S8" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="T8" s="75" t="s">
+      <c r="T8" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="110" t="s">
+      <c r="U8" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="V8" s="80" t="s">
+      <c r="V8" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="W8" s="82" t="s">
+      <c r="W8" s="104" t="s">
         <v>75</v>
       </c>
-      <c r="X8" s="98" t="s">
+      <c r="X8" s="84" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3497,61 +3497,61 @@
       <c r="B9" s="44">
         <v>12</v>
       </c>
-      <c r="C9" s="103"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="38" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="F9" s="39">
-        <v>44653.5</v>
+        <v>45384.5</v>
       </c>
       <c r="G9" s="39">
-        <v>44654.5</v>
+        <v>45385.5</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" s="84"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="87"/>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="107"/>
-      <c r="R9" s="109"/>
-      <c r="S9" s="76"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="111"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="83"/>
-      <c r="X9" s="88"/>
+        <v>92</v>
+      </c>
+      <c r="L9" s="106"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="107"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="110"/>
+      <c r="Q9" s="83"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="91"/>
+      <c r="V9" s="103"/>
+      <c r="W9" s="105"/>
+      <c r="X9" s="85"/>
     </row>
     <row r="10" spans="2:24" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="44">
         <v>13</v>
       </c>
-      <c r="C10" s="103"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="38" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="F10" s="39">
-        <v>44653.5</v>
+        <v>45384.5</v>
       </c>
       <c r="G10" s="39">
-        <v>44655.5</v>
+        <v>45386.5</v>
       </c>
       <c r="H10" s="38" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I10" s="38" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="L10" s="21">
         <f>SUM(M10:N10)</f>
@@ -3585,7 +3585,7 @@
       <c r="U10" s="22">
         <v>0</v>
       </c>
-      <c r="V10" s="112">
+      <c r="V10" s="46">
         <v>1</v>
       </c>
       <c r="W10" s="5" t="s">
@@ -3600,29 +3600,38 @@
       <c r="B11" s="45">
         <v>14</v>
       </c>
-      <c r="C11" s="104"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="40" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F11" s="41">
-        <v>44653.5</v>
+        <v>45384.5</v>
       </c>
       <c r="G11" s="41">
-        <v>44653.5</v>
+        <v>45384.5</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="I11" s="40" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="C6:C11"/>
     <mergeCell ref="L7:O7"/>
     <mergeCell ref="P7:Q7"/>
@@ -3631,13 +3640,6 @@
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="U8:U9"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="R7:V7"/>
     <mergeCell ref="V8:V9"/>
@@ -3646,8 +3648,6 @@
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="W7:X7"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3656,12 +3656,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3809,15 +3806,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3841,10 +3842,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>